<commit_message>
Changes sales returns storage from `PenerimaanBarang` into a new `ReturFaktur`.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_penjualan.xlsx
+++ b/test/integration/project/data_penjualan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -27,24 +27,21 @@
     <sheet name="BilyetGiro" sheetId="30" r:id="rId18"/>
     <sheet name="KewajibanPembayaran" sheetId="22" r:id="rId19"/>
     <sheet name="kewajibanpembayaran_items" sheetId="23" r:id="rId20"/>
-    <sheet name="FakturJual" sheetId="25" r:id="rId21"/>
-    <sheet name="PenerimaanBarang" sheetId="41" r:id="rId22"/>
-    <sheet name="PenerimaanBarang_items" sheetId="42" r:id="rId23"/>
+    <sheet name="returfaktur" sheetId="43" r:id="rId21"/>
+    <sheet name="returfaktur_items" sheetId="44" r:id="rId22"/>
+    <sheet name="FakturJual" sheetId="25" r:id="rId23"/>
     <sheet name="FakturJual_retur" sheetId="39" r:id="rId24"/>
     <sheet name="FakturJual_listItemFaktur" sheetId="26" r:id="rId25"/>
     <sheet name="PencairanPoin" sheetId="32" r:id="rId26"/>
     <sheet name="PencairanPoin_Items" sheetId="33" r:id="rId27"/>
     <sheet name="pesan" sheetId="37" r:id="rId28"/>
   </sheets>
-  <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="179">
   <si>
     <t>id</t>
   </si>
@@ -547,15 +544,6 @@
     <t>retur_ORDER</t>
   </si>
   <si>
-    <t>PO_ID</t>
-  </si>
-  <si>
-    <t>PO_ORDER</t>
-  </si>
-  <si>
-    <t>PenerimaanBarang_id</t>
-  </si>
-  <si>
     <t>Mr. New</t>
   </si>
   <si>
@@ -587,13 +575,16 @@
   </si>
   <si>
     <t>jumlahTukar</t>
+  </si>
+  <si>
+    <t>ReturFaktur_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -608,13 +599,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7D7D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -629,13 +632,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1763,7 +1767,7 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I5">
         <v>-1</v>
@@ -2246,7 +2250,7 @@
         <v>131</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H1" t="s">
         <v>58</v>
@@ -2279,6 +2283,97 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:R8"/>
@@ -2618,108 +2713,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet22"/>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet31"/>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:IV65536"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2751,7 +2750,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:H8"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3130,7 +3129,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -3196,7 +3195,7 @@
         <v>20</v>
       </c>
       <c r="P1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -3580,7 +3579,7 @@
         <v>200</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H13">
         <v>60</v>
@@ -5074,25 +5073,25 @@
         <v>67</v>
       </c>
       <c r="F1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" t="s">
         <v>173</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>174</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>175</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>176</v>
-      </c>
-      <c r="J1" t="s">
-        <v>177</v>
-      </c>
-      <c r="K1" t="s">
-        <v>178</v>
-      </c>
-      <c r="L1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add button to perform bulk clearings.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_penjualan.xlsx
+++ b/test/integration/project/data_penjualan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="179">
   <si>
     <t>id</t>
   </si>
@@ -1301,8 +1301,8 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1389,11 +1389,23 @@
       <c r="D3" s="1">
         <v>41748</v>
       </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="1">
+        <v>41748</v>
+      </c>
       <c r="H3" s="1">
         <v>41749</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>117</v>
       </c>
       <c r="L3">
         <v>-3</v>
@@ -2382,8 +2394,8 @@
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5042,7 +5054,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>